<commit_message>
Upload Y4_B2526_General_&_Special_Internal_1_B2_reference_data.xlsx via attendance app
</commit_message>
<xml_diff>
--- a/reference_data/Y4_B2526_General_&_Special_Internal_1_B2_reference_data.xlsx
+++ b/reference_data/Y4_B2526_General_&_Special_Internal_1_B2_reference_data.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:41000001_{D1663237-9D7B-F948-96E9-7EEC252FCD6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sayed\reference_data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1DE2135-4BF8-4329-B7D6-4D303BFE784C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1585" uniqueCount="639">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1590" uniqueCount="639">
   <si>
     <t>Student ID</t>
   </si>
@@ -2332,20 +2337,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E319"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A307" workbookViewId="0">
-      <selection activeCell="A315" sqref="A315:A319"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H312" sqref="H312"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.97265625" customWidth="1"/>
-    <col min="2" max="2" width="46.9453125" customWidth="1"/>
-    <col min="3" max="3" width="7.93359375" customWidth="1"/>
-    <col min="4" max="4" width="6.9921875" customWidth="1"/>
-    <col min="5" max="5" width="50.04296875" customWidth="1"/>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="47" customWidth="1"/>
+    <col min="3" max="3" width="8" customWidth="1"/>
+    <col min="4" max="4" width="7" customWidth="1"/>
+    <col min="5" max="5" width="50" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2362,7 +2367,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -2379,7 +2384,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -2396,7 +2401,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -2413,7 +2418,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
@@ -2430,7 +2435,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
@@ -2447,7 +2452,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
@@ -2464,7 +2469,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
@@ -2481,7 +2486,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>22</v>
       </c>
@@ -2498,7 +2503,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
@@ -2515,7 +2520,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>26</v>
       </c>
@@ -2532,7 +2537,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>28</v>
       </c>
@@ -2549,7 +2554,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
@@ -2566,7 +2571,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>32</v>
       </c>
@@ -2583,7 +2588,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>34</v>
       </c>
@@ -2600,7 +2605,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>36</v>
       </c>
@@ -2617,7 +2622,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>38</v>
       </c>
@@ -2634,7 +2639,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>40</v>
       </c>
@@ -2651,7 +2656,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>42</v>
       </c>
@@ -2668,7 +2673,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>44</v>
       </c>
@@ -2685,7 +2690,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>46</v>
       </c>
@@ -2702,7 +2707,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>48</v>
       </c>
@@ -2719,7 +2724,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>50</v>
       </c>
@@ -2736,7 +2741,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>52</v>
       </c>
@@ -2753,7 +2758,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>54</v>
       </c>
@@ -2770,7 +2775,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>56</v>
       </c>
@@ -2787,7 +2792,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>58</v>
       </c>
@@ -2804,7 +2809,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>60</v>
       </c>
@@ -2821,7 +2826,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>62</v>
       </c>
@@ -2838,7 +2843,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>64</v>
       </c>
@@ -2855,7 +2860,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>66</v>
       </c>
@@ -2872,7 +2877,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>68</v>
       </c>
@@ -2889,7 +2894,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>70</v>
       </c>
@@ -2906,7 +2911,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>72</v>
       </c>
@@ -2923,7 +2928,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>74</v>
       </c>
@@ -2940,7 +2945,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>76</v>
       </c>
@@ -2957,7 +2962,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>78</v>
       </c>
@@ -2974,7 +2979,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>80</v>
       </c>
@@ -2991,7 +2996,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>82</v>
       </c>
@@ -3008,7 +3013,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>84</v>
       </c>
@@ -3025,7 +3030,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>86</v>
       </c>
@@ -3042,7 +3047,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>88</v>
       </c>
@@ -3059,7 +3064,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>90</v>
       </c>
@@ -3076,7 +3081,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>92</v>
       </c>
@@ -3093,7 +3098,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>94</v>
       </c>
@@ -3110,7 +3115,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>96</v>
       </c>
@@ -3127,7 +3132,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>98</v>
       </c>
@@ -3144,7 +3149,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>100</v>
       </c>
@@ -3161,7 +3166,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>102</v>
       </c>
@@ -3178,7 +3183,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>104</v>
       </c>
@@ -3195,7 +3200,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>106</v>
       </c>
@@ -3212,7 +3217,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>108</v>
       </c>
@@ -3229,7 +3234,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>110</v>
       </c>
@@ -3246,7 +3251,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>112</v>
       </c>
@@ -3263,7 +3268,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>114</v>
       </c>
@@ -3280,7 +3285,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>116</v>
       </c>
@@ -3297,7 +3302,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>118</v>
       </c>
@@ -3314,7 +3319,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>120</v>
       </c>
@@ -3331,7 +3336,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>122</v>
       </c>
@@ -3348,7 +3353,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>124</v>
       </c>
@@ -3365,7 +3370,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>126</v>
       </c>
@@ -3382,7 +3387,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>128</v>
       </c>
@@ -3399,7 +3404,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>130</v>
       </c>
@@ -3416,7 +3421,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>132</v>
       </c>
@@ -3433,7 +3438,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>134</v>
       </c>
@@ -3450,7 +3455,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>137</v>
       </c>
@@ -3467,7 +3472,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>139</v>
       </c>
@@ -3484,7 +3489,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>141</v>
       </c>
@@ -3501,7 +3506,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>143</v>
       </c>
@@ -3518,7 +3523,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>145</v>
       </c>
@@ -3535,7 +3540,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>147</v>
       </c>
@@ -3552,7 +3557,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>149</v>
       </c>
@@ -3569,7 +3574,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>151</v>
       </c>
@@ -3586,7 +3591,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>153</v>
       </c>
@@ -3603,7 +3608,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>155</v>
       </c>
@@ -3620,7 +3625,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>157</v>
       </c>
@@ -3637,7 +3642,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>159</v>
       </c>
@@ -3654,7 +3659,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>161</v>
       </c>
@@ -3671,7 +3676,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>163</v>
       </c>
@@ -3688,7 +3693,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>165</v>
       </c>
@@ -3705,7 +3710,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>167</v>
       </c>
@@ -3722,7 +3727,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>169</v>
       </c>
@@ -3739,7 +3744,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>171</v>
       </c>
@@ -3756,7 +3761,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>173</v>
       </c>
@@ -3773,7 +3778,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>175</v>
       </c>
@@ -3790,7 +3795,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>177</v>
       </c>
@@ -3807,7 +3812,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>179</v>
       </c>
@@ -3824,7 +3829,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>181</v>
       </c>
@@ -3841,7 +3846,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>183</v>
       </c>
@@ -3858,7 +3863,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>185</v>
       </c>
@@ -3875,7 +3880,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>187</v>
       </c>
@@ -3892,7 +3897,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>189</v>
       </c>
@@ -3909,7 +3914,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>191</v>
       </c>
@@ -3926,7 +3931,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>193</v>
       </c>
@@ -3943,7 +3948,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>195</v>
       </c>
@@ -3960,7 +3965,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>197</v>
       </c>
@@ -3977,7 +3982,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>199</v>
       </c>
@@ -3994,7 +3999,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>201</v>
       </c>
@@ -4011,7 +4016,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
         <v>203</v>
       </c>
@@ -4028,7 +4033,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>205</v>
       </c>
@@ -4045,7 +4050,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>207</v>
       </c>
@@ -4062,7 +4067,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>209</v>
       </c>
@@ -4079,7 +4084,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
         <v>211</v>
       </c>
@@ -4096,7 +4101,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>213</v>
       </c>
@@ -4113,7 +4118,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
         <v>215</v>
       </c>
@@ -4130,7 +4135,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>217</v>
       </c>
@@ -4147,7 +4152,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
         <v>219</v>
       </c>
@@ -4164,7 +4169,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>221</v>
       </c>
@@ -4181,7 +4186,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
         <v>223</v>
       </c>
@@ -4198,7 +4203,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>225</v>
       </c>
@@ -4215,7 +4220,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
         <v>227</v>
       </c>
@@ -4232,7 +4237,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>229</v>
       </c>
@@ -4249,7 +4254,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
         <v>231</v>
       </c>
@@ -4266,7 +4271,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>233</v>
       </c>
@@ -4283,7 +4288,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
         <v>235</v>
       </c>
@@ -4300,7 +4305,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>237</v>
       </c>
@@ -4317,7 +4322,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
         <v>239</v>
       </c>
@@ -4334,7 +4339,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>241</v>
       </c>
@@ -4351,7 +4356,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
         <v>243</v>
       </c>
@@ -4368,7 +4373,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>245</v>
       </c>
@@ -4385,7 +4390,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
         <v>247</v>
       </c>
@@ -4402,7 +4407,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>249</v>
       </c>
@@ -4419,7 +4424,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
         <v>251</v>
       </c>
@@ -4436,7 +4441,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>253</v>
       </c>
@@ -4453,7 +4458,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
         <v>255</v>
       </c>
@@ -4470,7 +4475,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>257</v>
       </c>
@@ -4487,7 +4492,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
         <v>260</v>
       </c>
@@ -4504,7 +4509,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>262</v>
       </c>
@@ -4521,7 +4526,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
         <v>264</v>
       </c>
@@ -4538,7 +4543,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>266</v>
       </c>
@@ -4555,7 +4560,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
         <v>268</v>
       </c>
@@ -4572,7 +4577,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>270</v>
       </c>
@@ -4589,7 +4594,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
         <v>272</v>
       </c>
@@ -4606,7 +4611,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>274</v>
       </c>
@@ -4623,7 +4628,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
         <v>276</v>
       </c>
@@ -4640,7 +4645,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>278</v>
       </c>
@@ -4657,7 +4662,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
         <v>280</v>
       </c>
@@ -4674,7 +4679,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>282</v>
       </c>
@@ -4691,7 +4696,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
         <v>284</v>
       </c>
@@ -4708,7 +4713,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>286</v>
       </c>
@@ -4725,7 +4730,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
         <v>288</v>
       </c>
@@ -4742,7 +4747,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
         <v>290</v>
       </c>
@@ -4759,7 +4764,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
         <v>292</v>
       </c>
@@ -4776,7 +4781,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
         <v>294</v>
       </c>
@@ -4793,7 +4798,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
         <v>296</v>
       </c>
@@ -4810,7 +4815,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>298</v>
       </c>
@@ -4827,7 +4832,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
         <v>300</v>
       </c>
@@ -4844,7 +4849,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
         <v>302</v>
       </c>
@@ -4861,7 +4866,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
         <v>304</v>
       </c>
@@ -4878,7 +4883,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>306</v>
       </c>
@@ -4895,7 +4900,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="s">
         <v>308</v>
       </c>
@@ -4912,7 +4917,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>310</v>
       </c>
@@ -4929,7 +4934,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="s">
         <v>312</v>
       </c>
@@ -4946,7 +4951,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>314</v>
       </c>
@@ -4963,7 +4968,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
         <v>316</v>
       </c>
@@ -4980,7 +4985,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
         <v>318</v>
       </c>
@@ -4997,7 +5002,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
         <v>320</v>
       </c>
@@ -5014,7 +5019,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
         <v>322</v>
       </c>
@@ -5031,7 +5036,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
         <v>324</v>
       </c>
@@ -5048,7 +5053,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
         <v>326</v>
       </c>
@@ -5065,7 +5070,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
         <v>328</v>
       </c>
@@ -5082,7 +5087,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
         <v>330</v>
       </c>
@@ -5099,7 +5104,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
         <v>332</v>
       </c>
@@ -5116,7 +5121,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
         <v>334</v>
       </c>
@@ -5133,7 +5138,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="s">
         <v>336</v>
       </c>
@@ -5150,7 +5155,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
         <v>338</v>
       </c>
@@ -5167,7 +5172,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
         <v>340</v>
       </c>
@@ -5184,7 +5189,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
         <v>342</v>
       </c>
@@ -5201,7 +5206,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="3" t="s">
         <v>344</v>
       </c>
@@ -5218,7 +5223,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
         <v>346</v>
       </c>
@@ -5235,7 +5240,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="3" t="s">
         <v>348</v>
       </c>
@@ -5252,7 +5257,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
         <v>350</v>
       </c>
@@ -5269,7 +5274,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="3" t="s">
         <v>352</v>
       </c>
@@ -5286,7 +5291,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
         <v>354</v>
       </c>
@@ -5303,7 +5308,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="3" t="s">
         <v>356</v>
       </c>
@@ -5320,7 +5325,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
         <v>358</v>
       </c>
@@ -5337,7 +5342,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="s">
         <v>360</v>
       </c>
@@ -5354,7 +5359,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
         <v>362</v>
       </c>
@@ -5371,7 +5376,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="3" t="s">
         <v>364</v>
       </c>
@@ -5388,7 +5393,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
         <v>366</v>
       </c>
@@ -5405,7 +5410,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="3" t="s">
         <v>368</v>
       </c>
@@ -5422,7 +5427,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
         <v>370</v>
       </c>
@@ -5439,7 +5444,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="3" t="s">
         <v>372</v>
       </c>
@@ -5456,7 +5461,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
         <v>374</v>
       </c>
@@ -5473,7 +5478,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="3" t="s">
         <v>376</v>
       </c>
@@ -5490,7 +5495,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
         <v>378</v>
       </c>
@@ -5507,7 +5512,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="3" t="s">
         <v>380</v>
       </c>
@@ -5524,7 +5529,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
         <v>382</v>
       </c>
@@ -5541,7 +5546,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="3" t="s">
         <v>384</v>
       </c>
@@ -5558,7 +5563,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
         <v>386</v>
       </c>
@@ -5575,7 +5580,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" s="3" t="s">
         <v>389</v>
       </c>
@@ -5592,7 +5597,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
         <v>391</v>
       </c>
@@ -5609,7 +5614,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="3" t="s">
         <v>393</v>
       </c>
@@ -5626,7 +5631,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
         <v>395</v>
       </c>
@@ -5643,7 +5648,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" s="3" t="s">
         <v>397</v>
       </c>
@@ -5660,7 +5665,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
         <v>399</v>
       </c>
@@ -5677,7 +5682,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" s="3" t="s">
         <v>401</v>
       </c>
@@ -5694,7 +5699,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
         <v>403</v>
       </c>
@@ -5711,7 +5716,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" s="3" t="s">
         <v>405</v>
       </c>
@@ -5728,7 +5733,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
         <v>407</v>
       </c>
@@ -5745,7 +5750,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" s="3" t="s">
         <v>409</v>
       </c>
@@ -5762,7 +5767,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
         <v>411</v>
       </c>
@@ -5779,7 +5784,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" s="3" t="s">
         <v>413</v>
       </c>
@@ -5796,7 +5801,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
         <v>415</v>
       </c>
@@ -5813,7 +5818,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="3" t="s">
         <v>417</v>
       </c>
@@ -5830,7 +5835,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
         <v>419</v>
       </c>
@@ -5847,7 +5852,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="3" t="s">
         <v>421</v>
       </c>
@@ -5864,7 +5869,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
         <v>423</v>
       </c>
@@ -5881,7 +5886,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" s="3" t="s">
         <v>425</v>
       </c>
@@ -5898,7 +5903,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
         <v>427</v>
       </c>
@@ -5915,7 +5920,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" s="3" t="s">
         <v>429</v>
       </c>
@@ -5932,7 +5937,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
         <v>431</v>
       </c>
@@ -5949,7 +5954,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" s="3" t="s">
         <v>433</v>
       </c>
@@ -5966,7 +5971,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
         <v>435</v>
       </c>
@@ -5983,7 +5988,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" s="3" t="s">
         <v>437</v>
       </c>
@@ -6000,7 +6005,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
         <v>439</v>
       </c>
@@ -6017,7 +6022,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" s="3" t="s">
         <v>441</v>
       </c>
@@ -6034,7 +6039,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
         <v>443</v>
       </c>
@@ -6051,7 +6056,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" s="3" t="s">
         <v>445</v>
       </c>
@@ -6068,7 +6073,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
         <v>447</v>
       </c>
@@ -6085,7 +6090,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" s="3" t="s">
         <v>449</v>
       </c>
@@ -6102,7 +6107,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
         <v>451</v>
       </c>
@@ -6119,7 +6124,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" s="3" t="s">
         <v>453</v>
       </c>
@@ -6136,7 +6141,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
         <v>455</v>
       </c>
@@ -6153,7 +6158,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" s="3" t="s">
         <v>457</v>
       </c>
@@ -6170,7 +6175,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
         <v>459</v>
       </c>
@@ -6187,7 +6192,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" s="3" t="s">
         <v>461</v>
       </c>
@@ -6204,7 +6209,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
         <v>463</v>
       </c>
@@ -6221,7 +6226,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" s="3" t="s">
         <v>465</v>
       </c>
@@ -6238,7 +6243,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
         <v>467</v>
       </c>
@@ -6255,7 +6260,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" s="3" t="s">
         <v>469</v>
       </c>
@@ -6272,7 +6277,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" s="2" t="s">
         <v>471</v>
       </c>
@@ -6289,7 +6294,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" s="3" t="s">
         <v>473</v>
       </c>
@@ -6306,7 +6311,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
         <v>475</v>
       </c>
@@ -6323,7 +6328,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" s="3" t="s">
         <v>477</v>
       </c>
@@ -6340,7 +6345,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" s="2" t="s">
         <v>479</v>
       </c>
@@ -6357,7 +6362,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" s="3" t="s">
         <v>481</v>
       </c>
@@ -6374,7 +6379,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" s="2" t="s">
         <v>483</v>
       </c>
@@ -6391,7 +6396,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" s="3" t="s">
         <v>485</v>
       </c>
@@ -6408,7 +6413,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" s="2" t="s">
         <v>487</v>
       </c>
@@ -6425,7 +6430,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241" s="3" t="s">
         <v>489</v>
       </c>
@@ -6442,7 +6447,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" s="2" t="s">
         <v>491</v>
       </c>
@@ -6459,7 +6464,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" s="3" t="s">
         <v>493</v>
       </c>
@@ -6476,7 +6481,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
         <v>495</v>
       </c>
@@ -6493,7 +6498,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" s="3" t="s">
         <v>497</v>
       </c>
@@ -6510,7 +6515,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246" s="2" t="s">
         <v>499</v>
       </c>
@@ -6527,7 +6532,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247" s="3" t="s">
         <v>501</v>
       </c>
@@ -6544,7 +6549,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A248" s="2" t="s">
         <v>503</v>
       </c>
@@ -6561,7 +6566,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249" s="3" t="s">
         <v>505</v>
       </c>
@@ -6578,7 +6583,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250" s="2" t="s">
         <v>507</v>
       </c>
@@ -6595,7 +6600,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A251" s="3" t="s">
         <v>509</v>
       </c>
@@ -6612,7 +6617,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A252" s="2" t="s">
         <v>511</v>
       </c>
@@ -6629,7 +6634,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253" s="3" t="s">
         <v>514</v>
       </c>
@@ -6646,7 +6651,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" s="2" t="s">
         <v>516</v>
       </c>
@@ -6663,7 +6668,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A255" s="3" t="s">
         <v>518</v>
       </c>
@@ -6680,7 +6685,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A256" s="2" t="s">
         <v>520</v>
       </c>
@@ -6697,7 +6702,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257" s="3" t="s">
         <v>522</v>
       </c>
@@ -6714,7 +6719,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258" s="2" t="s">
         <v>524</v>
       </c>
@@ -6731,7 +6736,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" s="3" t="s">
         <v>526</v>
       </c>
@@ -6748,7 +6753,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
         <v>528</v>
       </c>
@@ -6765,7 +6770,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261" s="3" t="s">
         <v>530</v>
       </c>
@@ -6782,7 +6787,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" s="2" t="s">
         <v>532</v>
       </c>
@@ -6799,7 +6804,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" s="3" t="s">
         <v>534</v>
       </c>
@@ -6816,7 +6821,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" s="2" t="s">
         <v>536</v>
       </c>
@@ -6833,7 +6838,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" s="3" t="s">
         <v>538</v>
       </c>
@@ -6850,7 +6855,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266" s="2" t="s">
         <v>540</v>
       </c>
@@ -6867,7 +6872,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267" s="3" t="s">
         <v>542</v>
       </c>
@@ -6884,7 +6889,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A268" s="2" t="s">
         <v>544</v>
       </c>
@@ -6901,7 +6906,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269" s="3" t="s">
         <v>546</v>
       </c>
@@ -6918,7 +6923,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270" s="2" t="s">
         <v>548</v>
       </c>
@@ -6935,7 +6940,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" s="3" t="s">
         <v>550</v>
       </c>
@@ -6952,7 +6957,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272" s="2" t="s">
         <v>552</v>
       </c>
@@ -6969,7 +6974,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A273" s="3" t="s">
         <v>554</v>
       </c>
@@ -6986,7 +6991,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274" s="2" t="s">
         <v>556</v>
       </c>
@@ -7003,7 +7008,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A275" s="3" t="s">
         <v>558</v>
       </c>
@@ -7020,7 +7025,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A276" s="2" t="s">
         <v>560</v>
       </c>
@@ -7037,7 +7042,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A277" s="3" t="s">
         <v>562</v>
       </c>
@@ -7054,7 +7059,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A278" s="2" t="s">
         <v>564</v>
       </c>
@@ -7071,7 +7076,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A279" s="3" t="s">
         <v>566</v>
       </c>
@@ -7088,7 +7093,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A280" s="2" t="s">
         <v>568</v>
       </c>
@@ -7105,7 +7110,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A281" s="3" t="s">
         <v>570</v>
       </c>
@@ -7122,7 +7127,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A282" s="2" t="s">
         <v>572</v>
       </c>
@@ -7139,7 +7144,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A283" s="3" t="s">
         <v>574</v>
       </c>
@@ -7156,7 +7161,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A284" s="2" t="s">
         <v>576</v>
       </c>
@@ -7173,7 +7178,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A285" s="3" t="s">
         <v>578</v>
       </c>
@@ -7190,7 +7195,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A286" s="2" t="s">
         <v>580</v>
       </c>
@@ -7207,7 +7212,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A287" s="3" t="s">
         <v>582</v>
       </c>
@@ -7224,7 +7229,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A288" s="2" t="s">
         <v>584</v>
       </c>
@@ -7241,7 +7246,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A289" s="3" t="s">
         <v>586</v>
       </c>
@@ -7258,7 +7263,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A290" s="2" t="s">
         <v>588</v>
       </c>
@@ -7275,7 +7280,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A291" s="3" t="s">
         <v>590</v>
       </c>
@@ -7292,7 +7297,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A292" s="2" t="s">
         <v>592</v>
       </c>
@@ -7309,7 +7314,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A293" s="3" t="s">
         <v>594</v>
       </c>
@@ -7326,7 +7331,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A294" s="2" t="s">
         <v>596</v>
       </c>
@@ -7343,7 +7348,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A295" s="3" t="s">
         <v>598</v>
       </c>
@@ -7360,7 +7365,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A296" s="2" t="s">
         <v>600</v>
       </c>
@@ -7377,7 +7382,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A297" s="3" t="s">
         <v>602</v>
       </c>
@@ -7394,7 +7399,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A298" s="2" t="s">
         <v>604</v>
       </c>
@@ -7411,7 +7416,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A299" s="3" t="s">
         <v>606</v>
       </c>
@@ -7428,7 +7433,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A300" s="2" t="s">
         <v>608</v>
       </c>
@@ -7445,7 +7450,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A301" s="3" t="s">
         <v>610</v>
       </c>
@@ -7462,7 +7467,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A302" s="2" t="s">
         <v>612</v>
       </c>
@@ -7479,7 +7484,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A303" s="3" t="s">
         <v>614</v>
       </c>
@@ -7496,7 +7501,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A304" s="2" t="s">
         <v>616</v>
       </c>
@@ -7513,7 +7518,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A305" s="3" t="s">
         <v>618</v>
       </c>
@@ -7530,7 +7535,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A306" s="2" t="s">
         <v>620</v>
       </c>
@@ -7541,13 +7546,13 @@
         <v>7</v>
       </c>
       <c r="D306" s="2" t="s">
-        <v>513</v>
+        <v>8</v>
       </c>
       <c r="E306" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A307" s="3" t="s">
         <v>622</v>
       </c>
@@ -7558,13 +7563,13 @@
         <v>7</v>
       </c>
       <c r="D307" s="3" t="s">
-        <v>513</v>
+        <v>8</v>
       </c>
       <c r="E307" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A308" s="2" t="s">
         <v>624</v>
       </c>
@@ -7575,13 +7580,13 @@
         <v>7</v>
       </c>
       <c r="D308" s="2" t="s">
-        <v>513</v>
+        <v>8</v>
       </c>
       <c r="E308" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A309" s="3" t="s">
         <v>626</v>
       </c>
@@ -7598,7 +7603,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A310" s="2" t="s">
         <v>628</v>
       </c>
@@ -7615,7 +7620,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A311" s="3" t="s">
         <v>630</v>
       </c>
@@ -7632,7 +7637,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A312" s="2" t="s">
         <v>632</v>
       </c>
@@ -7649,7 +7654,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A313" s="3" t="s">
         <v>634</v>
       </c>
@@ -7666,7 +7671,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A314" s="2" t="s">
         <v>636</v>
       </c>
@@ -7683,74 +7688,89 @@
         <v>9</v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A315">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A315" s="2">
         <v>211892</v>
       </c>
-      <c r="B315" t="s">
+      <c r="B315" s="2" t="s">
         <v>638</v>
       </c>
-      <c r="C315" t="s">
-        <v>7</v>
-      </c>
-      <c r="D315" t="s">
+      <c r="C315" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D315" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A316">
+      <c r="E315" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A316" s="2">
         <v>211892</v>
       </c>
-      <c r="B316" t="s">
+      <c r="B316" s="2" t="s">
         <v>638</v>
       </c>
-      <c r="C316" t="s">
-        <v>7</v>
-      </c>
-      <c r="D316" t="s">
+      <c r="C316" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D316" s="2" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A317">
+      <c r="E316" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A317" s="2">
         <v>211892</v>
       </c>
-      <c r="B317" t="s">
+      <c r="B317" s="2" t="s">
         <v>638</v>
       </c>
-      <c r="C317" t="s">
-        <v>7</v>
-      </c>
-      <c r="D317" t="s">
+      <c r="C317" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D317" s="2" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A318">
+      <c r="E317" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A318" s="2">
         <v>211892</v>
       </c>
-      <c r="B318" t="s">
+      <c r="B318" s="2" t="s">
         <v>638</v>
       </c>
-      <c r="C318" t="s">
-        <v>7</v>
-      </c>
-      <c r="D318" t="s">
+      <c r="C318" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D318" s="2" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A319">
+      <c r="E318" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A319" s="2">
         <v>211892</v>
       </c>
-      <c r="B319" t="s">
+      <c r="B319" s="2" t="s">
         <v>638</v>
       </c>
-      <c r="C319" t="s">
-        <v>7</v>
-      </c>
-      <c r="D319" t="s">
+      <c r="C319" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D319" s="2" t="s">
         <v>513</v>
+      </c>
+      <c r="E319" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>